<commit_message>
code cleaned and packaged
</commit_message>
<xml_diff>
--- a/data/synthetic_sales_data.xlsx
+++ b/data/synthetic_sales_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Desktop\My portfolio content\LLM\Chatbot data analyst\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Desktop\My portfolio content\LLM\Chatbot data analyst\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9150F381-334B-431B-B47E-DE4041122CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D0C89B-2538-4EE0-BDA2-87A86EDEFCAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -95,6 +95,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -442,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>